<commit_message>
renamed repo, fixed output folder path
</commit_message>
<xml_diff>
--- a/outputs-HGR-r202-archive/c__Alphaproteobacteria.xlsx
+++ b/outputs-HGR-r202-archive/c__Alphaproteobacteria.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G160"/>
+  <dimension ref="A1:G134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,7 +503,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT11406.fa</t>
+          <t>even_MAG-GUT11468.fa</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -532,7 +532,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT11468.fa</t>
+          <t>even_MAG-GUT11535.fa</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -561,7 +561,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT11535.fa</t>
+          <t>even_MAG-GUT11596.fa</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -590,7 +590,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT11596.fa</t>
+          <t>even_MAG-GUT11640.fa</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -619,7 +619,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT11640.fa</t>
+          <t>even_MAG-GUT11729.fa</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -648,7 +648,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT11644.fa</t>
+          <t>even_MAG-GUT11931.fa</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -677,7 +677,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT11729.fa</t>
+          <t>even_MAG-GUT12173.fa</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -706,7 +706,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT11931.fa</t>
+          <t>even_MAG-GUT12225.fa</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -735,7 +735,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT12173.fa</t>
+          <t>even_MAG-GUT12256.fa</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -764,7 +764,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT12195.fa</t>
+          <t>even_MAG-GUT12267.fa</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -793,7 +793,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT12225.fa</t>
+          <t>even_MAG-GUT12348.fa</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -822,7 +822,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT12256.fa</t>
+          <t>even_MAG-GUT12377.fa</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -851,7 +851,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT12267.fa</t>
+          <t>even_MAG-GUT12481.fa</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -880,7 +880,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT12348.fa</t>
+          <t>even_MAG-GUT12789.fa</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -909,7 +909,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT12377.fa</t>
+          <t>even_MAG-GUT13549.fa</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -938,7 +938,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT12481.fa</t>
+          <t>even_MAG-GUT14112.fa</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -967,7 +967,7 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT12789.fa</t>
+          <t>even_MAG-GUT14915.fa</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -996,7 +996,7 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT13549.fa</t>
+          <t>even_MAG-GUT19089.fa</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1025,7 +1025,7 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT14112.fa</t>
+          <t>even_MAG-GUT23979.fa</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1054,7 +1054,7 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT14915.fa</t>
+          <t>even_MAG-GUT27476.fa</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1083,7 +1083,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT19089.fa</t>
+          <t>even_MAG-GUT27501.fa</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1112,7 +1112,7 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT2323.fa</t>
+          <t>even_MAG-GUT2752.fa</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1141,7 +1141,7 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT23979.fa</t>
+          <t>even_MAG-GUT27783.fa</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1170,7 +1170,7 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT2607.fa</t>
+          <t>even_MAG-GUT28018.fa</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -1199,7 +1199,7 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT27476.fa</t>
+          <t>even_MAG-GUT28028.fa</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -1228,7 +1228,7 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT27501.fa</t>
+          <t>even_MAG-GUT28206.fa</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -1257,7 +1257,7 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT2752.fa</t>
+          <t>even_MAG-GUT28651.fa</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1286,7 +1286,7 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT27781.fa</t>
+          <t>even_MAG-GUT28666.fa</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1315,7 +1315,7 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT27783.fa</t>
+          <t>even_MAG-GUT28677.fa</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1344,7 +1344,7 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT28018.fa</t>
+          <t>even_MAG-GUT28702.fa</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1373,7 +1373,7 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT28028.fa</t>
+          <t>even_MAG-GUT28960.fa</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1402,7 +1402,7 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT28206.fa</t>
+          <t>even_MAG-GUT28964.fa</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -1431,7 +1431,7 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT28651.fa</t>
+          <t>even_MAG-GUT28976.fa</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1460,7 +1460,7 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT28666.fa</t>
+          <t>even_MAG-GUT29001.fa</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1489,7 +1489,7 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT28677.fa</t>
+          <t>even_MAG-GUT29175.fa</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1518,7 +1518,7 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT28702.fa</t>
+          <t>even_MAG-GUT29239.fa</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1547,7 +1547,7 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT28960.fa</t>
+          <t>even_MAG-GUT2937.fa</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1576,7 +1576,7 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT28964.fa</t>
+          <t>even_MAG-GUT29515.fa</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1605,7 +1605,7 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT28976.fa</t>
+          <t>even_MAG-GUT29569.fa</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1634,7 +1634,7 @@
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT29001.fa</t>
+          <t>even_MAG-GUT31276.fa</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1663,7 +1663,7 @@
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT29175.fa</t>
+          <t>even_MAG-GUT31702.fa</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1692,7 +1692,7 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT29239.fa</t>
+          <t>even_MAG-GUT32803.fa</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1721,7 +1721,7 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT2937.fa</t>
+          <t>even_MAG-GUT37249.fa</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1750,7 +1750,7 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT29515.fa</t>
+          <t>even_MAG-GUT37818.fa</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1779,7 +1779,7 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT29569.fa</t>
+          <t>even_MAG-GUT39588.fa</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1808,7 +1808,7 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT31276.fa</t>
+          <t>even_MAG-GUT399.fa</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1837,7 +1837,7 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT31702.fa</t>
+          <t>even_MAG-GUT40004.fa</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1866,7 +1866,7 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT32803.fa</t>
+          <t>even_MAG-GUT40305.fa</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1895,7 +1895,7 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT37249.fa</t>
+          <t>even_MAG-GUT40499.fa</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1924,7 +1924,7 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT37559.fa</t>
+          <t>even_MAG-GUT40831.fa</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1953,7 +1953,7 @@
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT37818.fa</t>
+          <t>even_MAG-GUT42116.fa</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1982,7 +1982,7 @@
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT39588.fa</t>
+          <t>even_MAG-GUT42210.fa</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -2011,7 +2011,7 @@
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT399.fa</t>
+          <t>even_MAG-GUT42294.fa</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -2040,7 +2040,7 @@
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT40004.fa</t>
+          <t>even_MAG-GUT43269.fa</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -2069,7 +2069,7 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT40305.fa</t>
+          <t>even_MAG-GUT43691.fa</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -2098,7 +2098,7 @@
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT40499.fa</t>
+          <t>even_MAG-GUT44748.fa</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -2127,7 +2127,7 @@
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT40831.fa</t>
+          <t>even_MAG-GUT45352.fa</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -2156,7 +2156,7 @@
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT42116.fa</t>
+          <t>even_MAG-GUT45758.fa</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -2185,7 +2185,7 @@
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT42210.fa</t>
+          <t>even_MAG-GUT46039.fa</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -2214,7 +2214,7 @@
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT42294.fa</t>
+          <t>even_MAG-GUT48302.fa</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -2243,7 +2243,7 @@
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT43269.fa</t>
+          <t>even_MAG-GUT50003.fa</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -2272,7 +2272,7 @@
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT43691.fa</t>
+          <t>even_MAG-GUT50015.fa</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -2301,7 +2301,7 @@
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT44212.fa</t>
+          <t>even_MAG-GUT50866.fa</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -2330,7 +2330,7 @@
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT44748.fa</t>
+          <t>even_MAG-GUT50872.fa</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -2359,7 +2359,7 @@
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT44855.fa</t>
+          <t>even_MAG-GUT50906.fa</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -2388,7 +2388,7 @@
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT45352.fa</t>
+          <t>even_MAG-GUT50925.fa</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -2417,7 +2417,7 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT45758.fa</t>
+          <t>even_MAG-GUT50928.fa</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -2446,7 +2446,7 @@
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT46039.fa</t>
+          <t>even_MAG-GUT50936.fa</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -2475,7 +2475,7 @@
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT47176.fa</t>
+          <t>even_MAG-GUT53133.fa</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -2504,7 +2504,7 @@
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT48302.fa</t>
+          <t>even_MAG-GUT65550.fa</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -2533,7 +2533,7 @@
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT50003.fa</t>
+          <t>even_MAG-GUT65895.fa</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -2562,7 +2562,7 @@
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT50015.fa</t>
+          <t>even_MAG-GUT6623.fa</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -2591,7 +2591,7 @@
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT50121.fa</t>
+          <t>even_MAG-GUT66279.fa</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -2620,7 +2620,7 @@
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT50132.fa</t>
+          <t>even_MAG-GUT66843.fa</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -2649,7 +2649,7 @@
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT50866.fa</t>
+          <t>even_MAG-GUT66846.fa</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -2678,7 +2678,7 @@
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT50872.fa</t>
+          <t>even_MAG-GUT6708.fa</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -2707,7 +2707,7 @@
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT50906.fa</t>
+          <t>even_MAG-GUT67550.fa</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -2736,7 +2736,7 @@
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT50925.fa</t>
+          <t>even_MAG-GUT67681.fa</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -2765,7 +2765,7 @@
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT50928.fa</t>
+          <t>even_MAG-GUT67689.fa</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -2794,7 +2794,7 @@
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT50936.fa</t>
+          <t>even_MAG-GUT68091.fa</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -2823,7 +2823,7 @@
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT52916.fa</t>
+          <t>even_MAG-GUT68308.fa</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -2852,7 +2852,7 @@
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT52923.fa</t>
+          <t>even_MAG-GUT68561.fa</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -2881,7 +2881,7 @@
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT52941.fa</t>
+          <t>even_MAG-GUT68780.fa</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -2910,7 +2910,7 @@
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT53133.fa</t>
+          <t>even_MAG-GUT69595.fa</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -2939,7 +2939,7 @@
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT53142.fa</t>
+          <t>even_MAG-GUT69640.fa</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -2968,7 +2968,7 @@
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT65550.fa</t>
+          <t>even_MAG-GUT69665.fa</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -2997,7 +2997,7 @@
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT65895.fa</t>
+          <t>even_MAG-GUT69729.fa</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -3026,7 +3026,7 @@
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT6619.fa</t>
+          <t>even_MAG-GUT70973.fa</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -3055,7 +3055,7 @@
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT6623.fa</t>
+          <t>even_MAG-GUT71390.fa</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -3084,7 +3084,7 @@
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT66279.fa</t>
+          <t>even_MAG-GUT72079.fa</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -3113,7 +3113,7 @@
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT66843.fa</t>
+          <t>even_MAG-GUT72100.fa</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -3142,7 +3142,7 @@
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT66846.fa</t>
+          <t>even_MAG-GUT72283.fa</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -3171,7 +3171,7 @@
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT6708.fa</t>
+          <t>even_MAG-GUT72571.fa</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -3200,7 +3200,7 @@
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT6722.fa</t>
+          <t>even_MAG-GUT72585.fa</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -3229,7 +3229,7 @@
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT67367.fa</t>
+          <t>even_MAG-GUT72832.fa</t>
         </is>
       </c>
       <c r="B97" t="n">
@@ -3258,7 +3258,7 @@
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT67550.fa</t>
+          <t>even_MAG-GUT72841.fa</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -3287,7 +3287,7 @@
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT67681.fa</t>
+          <t>even_MAG-GUT73024.fa</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -3316,7 +3316,7 @@
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT67689.fa</t>
+          <t>even_MAG-GUT73734.fa</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -3345,7 +3345,7 @@
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT68091.fa</t>
+          <t>even_MAG-GUT73909.fa</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -3374,7 +3374,7 @@
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT68308.fa</t>
+          <t>even_MAG-GUT73910.fa</t>
         </is>
       </c>
       <c r="B102" t="n">
@@ -3403,7 +3403,7 @@
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT68561.fa</t>
+          <t>even_MAG-GUT74302.fa</t>
         </is>
       </c>
       <c r="B103" t="n">
@@ -3432,7 +3432,7 @@
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT6873.fa</t>
+          <t>even_MAG-GUT74323.fa</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -3461,7 +3461,7 @@
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT68780.fa</t>
+          <t>even_MAG-GUT74335.fa</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -3490,7 +3490,7 @@
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT69595.fa</t>
+          <t>even_MAG-GUT75478.fa</t>
         </is>
       </c>
       <c r="B106" t="n">
@@ -3519,7 +3519,7 @@
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT69640.fa</t>
+          <t>even_MAG-GUT76906.fa</t>
         </is>
       </c>
       <c r="B107" t="n">
@@ -3548,7 +3548,7 @@
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT69665.fa</t>
+          <t>even_MAG-GUT76981.fa</t>
         </is>
       </c>
       <c r="B108" t="n">
@@ -3577,7 +3577,7 @@
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT69729.fa</t>
+          <t>even_MAG-GUT76988.fa</t>
         </is>
       </c>
       <c r="B109" t="n">
@@ -3606,7 +3606,7 @@
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT70635.fa</t>
+          <t>even_MAG-GUT76995.fa</t>
         </is>
       </c>
       <c r="B110" t="n">
@@ -3635,7 +3635,7 @@
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT70973.fa</t>
+          <t>even_MAG-GUT77004.fa</t>
         </is>
       </c>
       <c r="B111" t="n">
@@ -3664,7 +3664,7 @@
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT71390.fa</t>
+          <t>even_MAG-GUT77348.fa</t>
         </is>
       </c>
       <c r="B112" t="n">
@@ -3693,7 +3693,7 @@
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT72079.fa</t>
+          <t>even_MAG-GUT77357.fa</t>
         </is>
       </c>
       <c r="B113" t="n">
@@ -3722,7 +3722,7 @@
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT72100.fa</t>
+          <t>even_MAG-GUT77371.fa</t>
         </is>
       </c>
       <c r="B114" t="n">
@@ -3751,7 +3751,7 @@
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT72283.fa</t>
+          <t>even_MAG-GUT77389.fa</t>
         </is>
       </c>
       <c r="B115" t="n">
@@ -3780,7 +3780,7 @@
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT72571.fa</t>
+          <t>even_MAG-GUT77514.fa</t>
         </is>
       </c>
       <c r="B116" t="n">
@@ -3809,7 +3809,7 @@
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT72585.fa</t>
+          <t>even_MAG-GUT77526.fa</t>
         </is>
       </c>
       <c r="B117" t="n">
@@ -3838,7 +3838,7 @@
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT72832.fa</t>
+          <t>even_MAG-GUT77839.fa</t>
         </is>
       </c>
       <c r="B118" t="n">
@@ -3867,7 +3867,7 @@
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT72841.fa</t>
+          <t>even_MAG-GUT82789.fa</t>
         </is>
       </c>
       <c r="B119" t="n">
@@ -3896,7 +3896,7 @@
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT73024.fa</t>
+          <t>even_MAG-GUT83640.fa</t>
         </is>
       </c>
       <c r="B120" t="n">
@@ -3925,7 +3925,7 @@
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT73734.fa</t>
+          <t>even_MAG-GUT83666.fa</t>
         </is>
       </c>
       <c r="B121" t="n">
@@ -3954,7 +3954,7 @@
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT73909.fa</t>
+          <t>even_MAG-GUT83683.fa</t>
         </is>
       </c>
       <c r="B122" t="n">
@@ -3983,7 +3983,7 @@
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT73910.fa</t>
+          <t>even_MAG-GUT84088.fa</t>
         </is>
       </c>
       <c r="B123" t="n">
@@ -4012,7 +4012,7 @@
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT74302.fa</t>
+          <t>even_MAG-GUT84361.fa</t>
         </is>
       </c>
       <c r="B124" t="n">
@@ -4041,7 +4041,7 @@
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT74323.fa</t>
+          <t>even_MAG-GUT84374.fa</t>
         </is>
       </c>
       <c r="B125" t="n">
@@ -4070,7 +4070,7 @@
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT74335.fa</t>
+          <t>even_MAG-GUT84479.fa</t>
         </is>
       </c>
       <c r="B126" t="n">
@@ -4099,7 +4099,7 @@
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT74695.fa</t>
+          <t>even_MAG-GUT85462.fa</t>
         </is>
       </c>
       <c r="B127" t="n">
@@ -4128,7 +4128,7 @@
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT75478.fa</t>
+          <t>even_MAG-GUT85601.fa</t>
         </is>
       </c>
       <c r="B128" t="n">
@@ -4157,7 +4157,7 @@
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT76906.fa</t>
+          <t>even_MAG-GUT85702.fa</t>
         </is>
       </c>
       <c r="B129" t="n">
@@ -4186,7 +4186,7 @@
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT76981.fa</t>
+          <t>even_MAG-GUT85992.fa</t>
         </is>
       </c>
       <c r="B130" t="n">
@@ -4215,7 +4215,7 @@
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT76988.fa</t>
+          <t>even_MAG-GUT86329.fa</t>
         </is>
       </c>
       <c r="B131" t="n">
@@ -4244,7 +4244,7 @@
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT76995.fa</t>
+          <t>even_MAG-GUT86341.fa</t>
         </is>
       </c>
       <c r="B132" t="n">
@@ -4273,7 +4273,7 @@
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT77004.fa</t>
+          <t>even_MAG-GUT86352.fa</t>
         </is>
       </c>
       <c r="B133" t="n">
@@ -4302,7 +4302,7 @@
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
         <is>
-          <t>even_MAG-GUT77348.fa</t>
+          <t>even_MAG-GUT86570.fa</t>
         </is>
       </c>
       <c r="B134" t="n">
@@ -4323,760 +4323,6 @@
         </is>
       </c>
       <c r="G134" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT77357.fa</t>
-        </is>
-      </c>
-      <c r="B135" t="n">
-        <v>1</v>
-      </c>
-      <c r="C135" t="n">
-        <v>0</v>
-      </c>
-      <c r="D135" t="n">
-        <v>0</v>
-      </c>
-      <c r="E135" t="n">
-        <v>1</v>
-      </c>
-      <c r="F135" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G135" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT77371.fa</t>
-        </is>
-      </c>
-      <c r="B136" t="n">
-        <v>1</v>
-      </c>
-      <c r="C136" t="n">
-        <v>0</v>
-      </c>
-      <c r="D136" t="n">
-        <v>0</v>
-      </c>
-      <c r="E136" t="n">
-        <v>1</v>
-      </c>
-      <c r="F136" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G136" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT77389.fa</t>
-        </is>
-      </c>
-      <c r="B137" t="n">
-        <v>1</v>
-      </c>
-      <c r="C137" t="n">
-        <v>0</v>
-      </c>
-      <c r="D137" t="n">
-        <v>0</v>
-      </c>
-      <c r="E137" t="n">
-        <v>1</v>
-      </c>
-      <c r="F137" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G137" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT77514.fa</t>
-        </is>
-      </c>
-      <c r="B138" t="n">
-        <v>1</v>
-      </c>
-      <c r="C138" t="n">
-        <v>0</v>
-      </c>
-      <c r="D138" t="n">
-        <v>0</v>
-      </c>
-      <c r="E138" t="n">
-        <v>1</v>
-      </c>
-      <c r="F138" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G138" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT77526.fa</t>
-        </is>
-      </c>
-      <c r="B139" t="n">
-        <v>1</v>
-      </c>
-      <c r="C139" t="n">
-        <v>0</v>
-      </c>
-      <c r="D139" t="n">
-        <v>0</v>
-      </c>
-      <c r="E139" t="n">
-        <v>1</v>
-      </c>
-      <c r="F139" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G139" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT77839.fa</t>
-        </is>
-      </c>
-      <c r="B140" t="n">
-        <v>1</v>
-      </c>
-      <c r="C140" t="n">
-        <v>0</v>
-      </c>
-      <c r="D140" t="n">
-        <v>0</v>
-      </c>
-      <c r="E140" t="n">
-        <v>1</v>
-      </c>
-      <c r="F140" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G140" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT78207.fa</t>
-        </is>
-      </c>
-      <c r="B141" t="n">
-        <v>1</v>
-      </c>
-      <c r="C141" t="n">
-        <v>0</v>
-      </c>
-      <c r="D141" t="n">
-        <v>0</v>
-      </c>
-      <c r="E141" t="n">
-        <v>1</v>
-      </c>
-      <c r="F141" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G141" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT79180.fa</t>
-        </is>
-      </c>
-      <c r="B142" t="n">
-        <v>1</v>
-      </c>
-      <c r="C142" t="n">
-        <v>0</v>
-      </c>
-      <c r="D142" t="n">
-        <v>0</v>
-      </c>
-      <c r="E142" t="n">
-        <v>1</v>
-      </c>
-      <c r="F142" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G142" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT82789.fa</t>
-        </is>
-      </c>
-      <c r="B143" t="n">
-        <v>1</v>
-      </c>
-      <c r="C143" t="n">
-        <v>0</v>
-      </c>
-      <c r="D143" t="n">
-        <v>0</v>
-      </c>
-      <c r="E143" t="n">
-        <v>1</v>
-      </c>
-      <c r="F143" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G143" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT83636.fa</t>
-        </is>
-      </c>
-      <c r="B144" t="n">
-        <v>1</v>
-      </c>
-      <c r="C144" t="n">
-        <v>0</v>
-      </c>
-      <c r="D144" t="n">
-        <v>0</v>
-      </c>
-      <c r="E144" t="n">
-        <v>1</v>
-      </c>
-      <c r="F144" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G144" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT83640.fa</t>
-        </is>
-      </c>
-      <c r="B145" t="n">
-        <v>1</v>
-      </c>
-      <c r="C145" t="n">
-        <v>0</v>
-      </c>
-      <c r="D145" t="n">
-        <v>0</v>
-      </c>
-      <c r="E145" t="n">
-        <v>1</v>
-      </c>
-      <c r="F145" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G145" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT83666.fa</t>
-        </is>
-      </c>
-      <c r="B146" t="n">
-        <v>1</v>
-      </c>
-      <c r="C146" t="n">
-        <v>0</v>
-      </c>
-      <c r="D146" t="n">
-        <v>0</v>
-      </c>
-      <c r="E146" t="n">
-        <v>1</v>
-      </c>
-      <c r="F146" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G146" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT83683.fa</t>
-        </is>
-      </c>
-      <c r="B147" t="n">
-        <v>1</v>
-      </c>
-      <c r="C147" t="n">
-        <v>0</v>
-      </c>
-      <c r="D147" t="n">
-        <v>0</v>
-      </c>
-      <c r="E147" t="n">
-        <v>1</v>
-      </c>
-      <c r="F147" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G147" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT840.fa</t>
-        </is>
-      </c>
-      <c r="B148" t="n">
-        <v>1</v>
-      </c>
-      <c r="C148" t="n">
-        <v>0</v>
-      </c>
-      <c r="D148" t="n">
-        <v>0</v>
-      </c>
-      <c r="E148" t="n">
-        <v>1</v>
-      </c>
-      <c r="F148" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G148" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT84088.fa</t>
-        </is>
-      </c>
-      <c r="B149" t="n">
-        <v>1</v>
-      </c>
-      <c r="C149" t="n">
-        <v>0</v>
-      </c>
-      <c r="D149" t="n">
-        <v>0</v>
-      </c>
-      <c r="E149" t="n">
-        <v>1</v>
-      </c>
-      <c r="F149" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G149" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT84361.fa</t>
-        </is>
-      </c>
-      <c r="B150" t="n">
-        <v>1</v>
-      </c>
-      <c r="C150" t="n">
-        <v>0</v>
-      </c>
-      <c r="D150" t="n">
-        <v>0</v>
-      </c>
-      <c r="E150" t="n">
-        <v>1</v>
-      </c>
-      <c r="F150" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G150" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT84374.fa</t>
-        </is>
-      </c>
-      <c r="B151" t="n">
-        <v>1</v>
-      </c>
-      <c r="C151" t="n">
-        <v>0</v>
-      </c>
-      <c r="D151" t="n">
-        <v>0</v>
-      </c>
-      <c r="E151" t="n">
-        <v>1</v>
-      </c>
-      <c r="F151" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G151" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT84479.fa</t>
-        </is>
-      </c>
-      <c r="B152" t="n">
-        <v>1</v>
-      </c>
-      <c r="C152" t="n">
-        <v>0</v>
-      </c>
-      <c r="D152" t="n">
-        <v>0</v>
-      </c>
-      <c r="E152" t="n">
-        <v>1</v>
-      </c>
-      <c r="F152" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G152" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT85462.fa</t>
-        </is>
-      </c>
-      <c r="B153" t="n">
-        <v>1</v>
-      </c>
-      <c r="C153" t="n">
-        <v>0</v>
-      </c>
-      <c r="D153" t="n">
-        <v>0</v>
-      </c>
-      <c r="E153" t="n">
-        <v>1</v>
-      </c>
-      <c r="F153" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G153" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT85601.fa</t>
-        </is>
-      </c>
-      <c r="B154" t="n">
-        <v>1</v>
-      </c>
-      <c r="C154" t="n">
-        <v>0</v>
-      </c>
-      <c r="D154" t="n">
-        <v>0</v>
-      </c>
-      <c r="E154" t="n">
-        <v>1</v>
-      </c>
-      <c r="F154" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G154" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT85702.fa</t>
-        </is>
-      </c>
-      <c r="B155" t="n">
-        <v>1</v>
-      </c>
-      <c r="C155" t="n">
-        <v>0</v>
-      </c>
-      <c r="D155" t="n">
-        <v>0</v>
-      </c>
-      <c r="E155" t="n">
-        <v>1</v>
-      </c>
-      <c r="F155" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G155" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT85992.fa</t>
-        </is>
-      </c>
-      <c r="B156" t="n">
-        <v>1</v>
-      </c>
-      <c r="C156" t="n">
-        <v>0</v>
-      </c>
-      <c r="D156" t="n">
-        <v>0</v>
-      </c>
-      <c r="E156" t="n">
-        <v>1</v>
-      </c>
-      <c r="F156" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G156" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT86329.fa</t>
-        </is>
-      </c>
-      <c r="B157" t="n">
-        <v>1</v>
-      </c>
-      <c r="C157" t="n">
-        <v>0</v>
-      </c>
-      <c r="D157" t="n">
-        <v>0</v>
-      </c>
-      <c r="E157" t="n">
-        <v>1</v>
-      </c>
-      <c r="F157" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G157" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT86341.fa</t>
-        </is>
-      </c>
-      <c r="B158" t="n">
-        <v>1</v>
-      </c>
-      <c r="C158" t="n">
-        <v>0</v>
-      </c>
-      <c r="D158" t="n">
-        <v>0</v>
-      </c>
-      <c r="E158" t="n">
-        <v>1</v>
-      </c>
-      <c r="F158" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G158" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT86352.fa</t>
-        </is>
-      </c>
-      <c r="B159" t="n">
-        <v>1</v>
-      </c>
-      <c r="C159" t="n">
-        <v>0</v>
-      </c>
-      <c r="D159" t="n">
-        <v>0</v>
-      </c>
-      <c r="E159" t="n">
-        <v>1</v>
-      </c>
-      <c r="F159" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G159" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" s="1" t="inlineStr">
-        <is>
-          <t>even_MAG-GUT86570.fa</t>
-        </is>
-      </c>
-      <c r="B160" t="n">
-        <v>1</v>
-      </c>
-      <c r="C160" t="n">
-        <v>0</v>
-      </c>
-      <c r="D160" t="n">
-        <v>0</v>
-      </c>
-      <c r="E160" t="n">
-        <v>1</v>
-      </c>
-      <c r="F160" t="inlineStr">
-        <is>
-          <t>o__RF32</t>
-        </is>
-      </c>
-      <c r="G160" t="inlineStr">
         <is>
           <t>o__RF32</t>
         </is>

</xml_diff>